<commit_message>
Added the following page testcases listing page, project overview page, shopping page
</commit_message>
<xml_diff>
--- a/src/main/java/com/demo/automation/POMFramework/data/TestData.xlsx
+++ b/src/main/java/com/demo/automation/POMFramework/data/TestData.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsingh5/git/POMWithPageFactoryFramework/src/main/java/com/test/automation/uiAutomation/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1215" windowWidth="14295" windowHeight="3540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>userName</t>
   </si>
@@ -45,13 +41,19 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>jakay34@gmail.com</t>
+  </si>
+  <si>
+    <t>12345678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,10 +105,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -165,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -200,7 +203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -377,26 +380,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -407,7 +410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -418,7 +421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -429,7 +432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -440,7 +443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -451,7 +454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -462,7 +465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -473,12 +476,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Added the testNg suite file and added two more test cases.
</commit_message>
<xml_diff>
--- a/src/main/java/com/demo/automation/POMFramework/data/TestData.xlsx
+++ b/src/main/java/com/demo/automation/POMFramework/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1215" windowWidth="14295" windowHeight="3540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1215" windowWidth="19815" windowHeight="3540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>userName</t>
   </si>
@@ -34,9 +34,6 @@
     <t>runMode</t>
   </si>
   <si>
-    <t>automation@gmail.com</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -47,6 +44,24 @@
   </si>
   <si>
     <t>12345678</t>
+  </si>
+  <si>
+    <t>jakay11@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay12@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay13@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay14@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay15@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay16@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -380,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,7 +406,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -412,90 +427,90 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>12345678</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>12345678</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>12345678</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>12345678</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>12345678</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A8" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="A4" r:id="rId6"/>
+    <hyperlink ref="A5" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pom.xml added the send Mail report through maven and added the bat file
</commit_message>
<xml_diff>
--- a/src/main/java/com/demo/automation/POMFramework/data/TestData.xlsx
+++ b/src/main/java/com/demo/automation/POMFramework/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1215" windowWidth="19815" windowHeight="3540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>jakay34@gmail.com</t>
   </si>
   <si>
-    <t>12345678</t>
-  </si>
-  <si>
     <t>jakay11@gmail.com</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>jakay16@gmail.com</t>
+  </si>
+  <si>
+    <t>wqerewr</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -427,7 +427,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>12345678</v>
@@ -438,10 +438,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>12345678</v>
+        <v>12345</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -449,10 +449,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>12345678</v>
+        <v>1378</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -460,10 +460,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>12345678</v>
+        <v>12678</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>12345678</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>12345678</v>
@@ -496,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>

</xml_diff>